<commit_message>
cierre 25 mar 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/TURNOS CENTRAL.xlsx
+++ b/01 DOCUEMENTOS/TURNOS CENTRAL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t xml:space="preserve">CONTROL DE TURNOS CENTRAL </t>
   </si>
@@ -508,7 +508,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="H2" s="5">
-        <v>44530</v>
+        <v>44569</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="H5" s="5">
-        <v>44541</v>
+        <v>44588</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="H7" s="5">
-        <v>44569</v>
+        <v>44604</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="H8" t="s">
+      <c r="H8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -609,6 +609,9 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -618,8 +621,8 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="H10" s="5">
-        <v>44588</v>
+      <c r="H10" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -630,8 +633,8 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="H11" t="s">
-        <v>5</v>
+      <c r="H11" s="5">
+        <v>44645</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -642,8 +645,8 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="H12" s="5">
-        <v>44604</v>
+      <c r="H12" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -654,9 +657,6 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="H13" s="6" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -666,9 +666,6 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="H14" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -678,9 +675,6 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="H15" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">

</xml_diff>